<commit_message>
Changed SNR formula and the value of SNR (still need to check constants!)
</commit_message>
<xml_diff>
--- a/puma_cat/psr_iar.xlsx
+++ b/puma_cat/psr_iar.xlsx
@@ -14,7 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="396">
+  <si>
+    <t>J0134-2937</t>
+  </si>
+  <si>
+    <t>J0255-5304</t>
+  </si>
+  <si>
+    <t>J0401-7608</t>
+  </si>
   <si>
     <t>J0437-4715</t>
   </si>
@@ -22,331 +31,1177 @@
     <t>J0452-1759</t>
   </si>
   <si>
+    <t>J0536-7543</t>
+  </si>
+  <si>
     <t>J0630-2834</t>
   </si>
   <si>
+    <t>J0656-2228</t>
+  </si>
+  <si>
+    <t>J0729-1836</t>
+  </si>
+  <si>
     <t>J0738-4042</t>
   </si>
   <si>
     <t>J0742-2822</t>
   </si>
   <si>
+    <t>J0745-5353</t>
+  </si>
+  <si>
+    <t>J0758-1528</t>
+  </si>
+  <si>
+    <t>J0809-4753</t>
+  </si>
+  <si>
+    <t>J0820-1350</t>
+  </si>
+  <si>
     <t>J0835-4510</t>
   </si>
   <si>
     <t>J0837-4135</t>
   </si>
   <si>
+    <t>J0846-3533</t>
+  </si>
+  <si>
+    <t>J0856-6137</t>
+  </si>
+  <si>
     <t>J0907-5157</t>
   </si>
   <si>
+    <t>J0908-1739</t>
+  </si>
+  <si>
     <t>J0908-4913</t>
   </si>
   <si>
+    <t>J0909-7212</t>
+  </si>
+  <si>
+    <t>J0924-5814</t>
+  </si>
+  <si>
+    <t>J0934-5249</t>
+  </si>
+  <si>
     <t>J0942-5552</t>
   </si>
   <si>
+    <t>J0952-3839</t>
+  </si>
+  <si>
+    <t>J1001-5507</t>
+  </si>
+  <si>
+    <t>J1012-5857</t>
+  </si>
+  <si>
+    <t>J1013-5934</t>
+  </si>
+  <si>
+    <t>J1017-5621</t>
+  </si>
+  <si>
+    <t>J1047-6709</t>
+  </si>
+  <si>
+    <t>J1048-5832</t>
+  </si>
+  <si>
     <t>J1056-6258</t>
   </si>
   <si>
+    <t>J1110-5637</t>
+  </si>
+  <si>
+    <t>J1114-6100</t>
+  </si>
+  <si>
+    <t>J1116-4122</t>
+  </si>
+  <si>
+    <t>J1117-6154</t>
+  </si>
+  <si>
+    <t>J1136-5525</t>
+  </si>
+  <si>
+    <t>J1141-6545</t>
+  </si>
+  <si>
     <t>J1157-6224</t>
   </si>
   <si>
+    <t>J1202-5820</t>
+  </si>
+  <si>
+    <t>J1210-5559</t>
+  </si>
+  <si>
+    <t>J1224-6407</t>
+  </si>
+  <si>
+    <t>J1225-6408</t>
+  </si>
+  <si>
     <t>J1243-6423</t>
   </si>
   <si>
+    <t>J1253-5820</t>
+  </si>
+  <si>
+    <t>J1306-6617</t>
+  </si>
+  <si>
+    <t>J1320-3512</t>
+  </si>
+  <si>
     <t>J1326-5859</t>
   </si>
   <si>
+    <t>J1326-6408</t>
+  </si>
+  <si>
     <t>J1326-6700</t>
   </si>
   <si>
     <t>J1327-6222</t>
   </si>
   <si>
+    <t>J1327-6301</t>
+  </si>
+  <si>
+    <t>J1328-4357</t>
+  </si>
+  <si>
+    <t>J1338-6204</t>
+  </si>
+  <si>
     <t>J1357-62</t>
   </si>
   <si>
     <t>J1359-6038</t>
   </si>
   <si>
+    <t>J1401-6357</t>
+  </si>
+  <si>
+    <t>J1410-7404</t>
+  </si>
+  <si>
+    <t>J1428-5530</t>
+  </si>
+  <si>
     <t>J1430-6623</t>
   </si>
   <si>
+    <t>J1452-6036</t>
+  </si>
+  <si>
     <t>J1453-6413</t>
   </si>
   <si>
     <t>J1456-6843</t>
   </si>
   <si>
+    <t>J1512-5759</t>
+  </si>
+  <si>
+    <t>J1522-5829</t>
+  </si>
+  <si>
+    <t>J1534-5334</t>
+  </si>
+  <si>
+    <t>J1539-5626</t>
+  </si>
+  <si>
+    <t>J1544-5308</t>
+  </si>
+  <si>
+    <t>J1557-4258</t>
+  </si>
+  <si>
     <t>J1559-4438</t>
   </si>
   <si>
     <t>J1600-5044</t>
   </si>
   <si>
+    <t>J1602-5100</t>
+  </si>
+  <si>
+    <t>J1604-4909</t>
+  </si>
+  <si>
     <t>J1605-5257</t>
   </si>
   <si>
+    <t>J1611-5209</t>
+  </si>
+  <si>
+    <t>J1614-5048</t>
+  </si>
+  <si>
+    <t>J1630-4733</t>
+  </si>
+  <si>
+    <t>J1633-4453</t>
+  </si>
+  <si>
+    <t>J1633-5015</t>
+  </si>
+  <si>
+    <t>J1643-1224</t>
+  </si>
+  <si>
     <t>J1644-4559</t>
   </si>
   <si>
+    <t>J1646-6831</t>
+  </si>
+  <si>
     <t>J1651-4246</t>
   </si>
   <si>
+    <t>J1651-5222</t>
+  </si>
+  <si>
+    <t>J1651-5255</t>
+  </si>
+  <si>
+    <t>J1653-3838</t>
+  </si>
+  <si>
+    <t>J1701-3726</t>
+  </si>
+  <si>
+    <t>J1703-3241</t>
+  </si>
+  <si>
+    <t>J1703-4851</t>
+  </si>
+  <si>
+    <t>J1705-3423</t>
+  </si>
+  <si>
     <t>J1707-4053</t>
   </si>
   <si>
+    <t>J1707-4729</t>
+  </si>
+  <si>
     <t>J1709-1640</t>
   </si>
   <si>
     <t>J1709-4429</t>
   </si>
   <si>
+    <t>J1717-3425</t>
+  </si>
+  <si>
     <t>J1721-3532</t>
   </si>
   <si>
+    <t>J1722-3207</t>
+  </si>
+  <si>
+    <t>J1722-3712</t>
+  </si>
+  <si>
+    <t>J1730-3350</t>
+  </si>
+  <si>
     <t>J1731-4744</t>
   </si>
   <si>
+    <t>J1733-3716</t>
+  </si>
+  <si>
+    <t>J1738-3211</t>
+  </si>
+  <si>
+    <t>J1739-2903</t>
+  </si>
+  <si>
+    <t>J1739-3131</t>
+  </si>
+  <si>
+    <t>J1740-3015</t>
+  </si>
+  <si>
+    <t>J1741-3927</t>
+  </si>
+  <si>
     <t>J1744-1134</t>
   </si>
   <si>
     <t>J1745-3040</t>
   </si>
   <si>
+    <t>J1750-3157</t>
+  </si>
+  <si>
+    <t>J1751-3323</t>
+  </si>
+  <si>
+    <t>J1751-4657</t>
+  </si>
+  <si>
     <t>J1752-2806</t>
   </si>
   <si>
+    <t>J1757-2421</t>
+  </si>
+  <si>
+    <t>J1803-2137</t>
+  </si>
+  <si>
+    <t>J1817-3618</t>
+  </si>
+  <si>
+    <t>J1817-3837</t>
+  </si>
+  <si>
+    <t>J1818-1422</t>
+  </si>
+  <si>
+    <t>J1822-2256</t>
+  </si>
+  <si>
+    <t>J1823-3106</t>
+  </si>
+  <si>
+    <t>J1824-1945</t>
+  </si>
+  <si>
+    <t>J1826-1334</t>
+  </si>
+  <si>
     <t>J1829-1751</t>
   </si>
   <si>
+    <t>J1830-1059</t>
+  </si>
+  <si>
+    <t>J1836-1008</t>
+  </si>
+  <si>
     <t>J1900-2600</t>
   </si>
   <si>
+    <t>J1941-2602</t>
+  </si>
+  <si>
     <t>J2048-1616</t>
   </si>
   <si>
+    <t>J2053-7200</t>
+  </si>
+  <si>
+    <t>J2241-5236</t>
+  </si>
+  <si>
+    <t>J2330-2005</t>
+  </si>
+  <si>
+    <t>01:34:18.6824</t>
+  </si>
+  <si>
+    <t>02:55:56.221</t>
+  </si>
+  <si>
+    <t>04:01:51.68</t>
+  </si>
+  <si>
     <t>04:37:15.8961737</t>
   </si>
   <si>
     <t>04:52:34.1057</t>
   </si>
   <si>
+    <t>05:36:30.79</t>
+  </si>
+  <si>
     <t>06:30:49.404393</t>
   </si>
   <si>
+    <t>06:56:30.207</t>
+  </si>
+  <si>
+    <t>07:29:32.3502</t>
+  </si>
+  <si>
     <t>07:38:32.329</t>
   </si>
   <si>
     <t>07:42:49.058</t>
   </si>
   <si>
+    <t>07:45:02.3</t>
+  </si>
+  <si>
+    <t>07:58:29.0708</t>
+  </si>
+  <si>
+    <t>08:09:43.890</t>
+  </si>
+  <si>
+    <t>08:20:26.3817</t>
+  </si>
+  <si>
     <t>08:35:20.61149</t>
   </si>
   <si>
     <t>08:37:21.1818</t>
   </si>
   <si>
+    <t>08:46:06.059</t>
+  </si>
+  <si>
+    <t>08:56:59.31</t>
+  </si>
+  <si>
     <t>09:07:15.900</t>
   </si>
   <si>
+    <t>09:08:38.1822</t>
+  </si>
+  <si>
     <t>09:08:35.53</t>
   </si>
   <si>
+    <t>09:09:36.0</t>
+  </si>
+  <si>
+    <t>09:24:31.0</t>
+  </si>
+  <si>
+    <t>09:34:28.30</t>
+  </si>
+  <si>
     <t>09:42:15.83</t>
   </si>
   <si>
+    <t>09:52:17.2</t>
+  </si>
+  <si>
+    <t>10:01:37.98</t>
+  </si>
+  <si>
+    <t>10:12:48.5</t>
+  </si>
+  <si>
+    <t>10:13:31.854</t>
+  </si>
+  <si>
+    <t>10:17:12.86</t>
+  </si>
+  <si>
+    <t>10:47:28.282</t>
+  </si>
+  <si>
+    <t>10:48:12.2</t>
+  </si>
+  <si>
     <t>10:56:25.55</t>
   </si>
   <si>
+    <t>11:10:00.40</t>
+  </si>
+  <si>
+    <t>11:14:22.52</t>
+  </si>
+  <si>
+    <t>11:16:43.086</t>
+  </si>
+  <si>
+    <t>11:17:23.81</t>
+  </si>
+  <si>
+    <t>11:36:02.17</t>
+  </si>
+  <si>
+    <t>11:41:07.0140</t>
+  </si>
+  <si>
     <t>11:57:15.240</t>
   </si>
   <si>
+    <t>12:02:28.403</t>
+  </si>
+  <si>
+    <t>12:10:05.988</t>
+  </si>
+  <si>
+    <t>12:24:22.185</t>
+  </si>
+  <si>
+    <t>12:25:42.8</t>
+  </si>
+  <si>
     <t>12:43:17.158</t>
   </si>
   <si>
+    <t>12:53:28.342</t>
+  </si>
+  <si>
+    <t>13:06:38.19</t>
+  </si>
+  <si>
+    <t>13:20:12.68</t>
+  </si>
+  <si>
     <t>13:26:58.27</t>
   </si>
   <si>
+    <t>13:26:32.4</t>
+  </si>
+  <si>
     <t>13:26:02.7</t>
   </si>
   <si>
     <t>13:27:17.4</t>
   </si>
   <si>
+    <t>13:27:07.47</t>
+  </si>
+  <si>
+    <t>13:28:06.432</t>
+  </si>
+  <si>
+    <t>13:38:09.35</t>
+  </si>
+  <si>
     <t>13:57:25</t>
   </si>
   <si>
     <t>13:59:58.22</t>
   </si>
   <si>
+    <t>14:01:52.48</t>
+  </si>
+  <si>
+    <t>14:10:07.370</t>
+  </si>
+  <si>
+    <t>14:28:26.297</t>
+  </si>
+  <si>
     <t>14:30:40.872</t>
   </si>
   <si>
+    <t>14:52:51.898</t>
+  </si>
+  <si>
     <t>14:53:32.737</t>
   </si>
   <si>
     <t>14:56:00.158</t>
   </si>
   <si>
+    <t>15:12:43.026</t>
+  </si>
+  <si>
+    <t>15:22:42.27</t>
+  </si>
+  <si>
+    <t>15:34:08.37</t>
+  </si>
+  <si>
+    <t>15:39:13.96</t>
+  </si>
+  <si>
+    <t>15:44:59.844</t>
+  </si>
+  <si>
+    <t>15:57:00.2580</t>
+  </si>
+  <si>
     <t>15:59:41.526126</t>
   </si>
   <si>
     <t>16:00:53.031</t>
   </si>
   <si>
+    <t>16:02:18.7</t>
+  </si>
+  <si>
+    <t>16:04:22.999</t>
+  </si>
+  <si>
     <t>16:05:16.2</t>
   </si>
   <si>
+    <t>16:11:03.20</t>
+  </si>
+  <si>
+    <t>16:14:11.29</t>
+  </si>
+  <si>
+    <t>16:30:37.47</t>
+  </si>
+  <si>
+    <t>16:33:47.048</t>
+  </si>
+  <si>
+    <t>16:33:00.103</t>
+  </si>
+  <si>
+    <t>16:43:38.1611</t>
+  </si>
+  <si>
     <t>16:44:49.281</t>
   </si>
   <si>
+    <t>16:46:54.8</t>
+  </si>
+  <si>
     <t>16:51:48.79</t>
   </si>
   <si>
+    <t>16:51:42.97</t>
+  </si>
+  <si>
+    <t>16:51:41.2</t>
+  </si>
+  <si>
+    <t>16:53:39.798</t>
+  </si>
+  <si>
+    <t>17:01:18.54</t>
+  </si>
+  <si>
+    <t>17:03:22.5406</t>
+  </si>
+  <si>
+    <t>17:03:54.40</t>
+  </si>
+  <si>
+    <t>17:05:42.363</t>
+  </si>
+  <si>
     <t>17:07:21.728</t>
   </si>
   <si>
+    <t>17:07:15.547</t>
+  </si>
+  <si>
     <t>17:09:26.4413</t>
   </si>
   <si>
     <t>17:09:42.728</t>
   </si>
   <si>
+    <t>17:17:20.2442</t>
+  </si>
+  <si>
     <t>17:21:32.7786</t>
   </si>
   <si>
+    <t>17:22:02.9547</t>
+  </si>
+  <si>
+    <t>17:22:59.17</t>
+  </si>
+  <si>
+    <t>17:30:32.5588</t>
+  </si>
+  <si>
     <t>17:31:42.103</t>
   </si>
   <si>
+    <t>17:33:26.7628</t>
+  </si>
+  <si>
+    <t>17:38:54.185</t>
+  </si>
+  <si>
+    <t>17:39:34.2777</t>
+  </si>
+  <si>
+    <t>17:39:24.3037</t>
+  </si>
+  <si>
+    <t>17:40:33.82</t>
+  </si>
+  <si>
+    <t>17:41:18.081</t>
+  </si>
+  <si>
     <t>17:44:29.4057891</t>
   </si>
   <si>
     <t>17:45:56.3127</t>
   </si>
   <si>
+    <t>17:50:47.3182</t>
+  </si>
+  <si>
+    <t>17:51:32.725</t>
+  </si>
+  <si>
+    <t>17:51:42.233</t>
+  </si>
+  <si>
     <t>17:52:58.6896</t>
   </si>
   <si>
+    <t>17:57:29.3231</t>
+  </si>
+  <si>
+    <t>18:03:51.4105</t>
+  </si>
+  <si>
+    <t>18:17:05.777</t>
+  </si>
+  <si>
+    <t>18:17:00.270</t>
+  </si>
+  <si>
+    <t>18:18:23.7660</t>
+  </si>
+  <si>
+    <t>18:22:58.9536</t>
+  </si>
+  <si>
+    <t>18:23:46.7881</t>
+  </si>
+  <si>
+    <t>18:24:00.4549</t>
+  </si>
+  <si>
+    <t>18:26:13.175</t>
+  </si>
+  <si>
     <t>18:29:43.1366</t>
   </si>
   <si>
+    <t>18:30:47.5662</t>
+  </si>
+  <si>
+    <t>18:36:53.9251</t>
+  </si>
+  <si>
     <t>19:00:47.582</t>
   </si>
   <si>
+    <t>19:41:00.4070</t>
+  </si>
+  <si>
     <t>20:48:35.640637</t>
   </si>
   <si>
+    <t>20:53:47.14</t>
+  </si>
+  <si>
+    <t>22:41:42.01850</t>
+  </si>
+  <si>
+    <t>23:30:26.885</t>
+  </si>
+  <si>
+    <t>-29:37:17.042</t>
+  </si>
+  <si>
+    <t>-53:04:21.36</t>
+  </si>
+  <si>
+    <t>-76:08:13.8</t>
+  </si>
+  <si>
     <t>-47:15:09.110714</t>
   </si>
   <si>
     <t>-17:59:23.371</t>
   </si>
   <si>
+    <t>-75:43:56.7</t>
+  </si>
+  <si>
     <t>-28:34:42.77881</t>
   </si>
   <si>
+    <t>-22:28:25.55</t>
+  </si>
+  <si>
+    <t>-18:36:42.7553</t>
+  </si>
+  <si>
     <t>-40:42:40.94</t>
   </si>
   <si>
     <t>-28:22:43.76</t>
   </si>
   <si>
+    <t>-53:51:22</t>
+  </si>
+  <si>
+    <t>-15:28:08.738</t>
+  </si>
+  <si>
+    <t>-47:53:55.14</t>
+  </si>
+  <si>
+    <t>-13:50:55.859</t>
+  </si>
+  <si>
     <t>-45:10:34.8751</t>
   </si>
   <si>
     <t>-41:35:14.37</t>
   </si>
   <si>
+    <t>-35:33:40.6632</t>
+  </si>
+  <si>
+    <t>-61:37:53.3</t>
+  </si>
+  <si>
     <t>-51:57:59.25</t>
   </si>
   <si>
+    <t>-17:39:37.67</t>
+  </si>
+  <si>
     <t>-49:13:06.5</t>
   </si>
   <si>
+    <t>-72:12:08.4</t>
+  </si>
+  <si>
+    <t>-58:14:06.4</t>
+  </si>
+  <si>
+    <t>-52:49:27.2</t>
+  </si>
+  <si>
     <t>-55:52:52.3</t>
   </si>
   <si>
+    <t>-38:39:10.2</t>
+  </si>
+  <si>
+    <t>-55:07:06.7</t>
+  </si>
+  <si>
+    <t>-58:57:48.7</t>
+  </si>
+  <si>
+    <t>-59:34:26.7</t>
+  </si>
+  <si>
+    <t>-56:21:30.7</t>
+  </si>
+  <si>
+    <t>-67:09:51.066</t>
+  </si>
+  <si>
+    <t>-58:32:05.8</t>
+  </si>
+  <si>
     <t>-62:58:47.6</t>
   </si>
   <si>
+    <t>-56:37:32.9</t>
+  </si>
+  <si>
+    <t>-61:00:34.2</t>
+  </si>
+  <si>
+    <t>-41:22:43.96</t>
+  </si>
+  <si>
+    <t>-61:54:22</t>
+  </si>
+  <si>
+    <t>-55:25:08.3</t>
+  </si>
+  <si>
+    <t>-65:45:19.1131</t>
+  </si>
+  <si>
     <t>-62:24:50.87</t>
   </si>
   <si>
+    <t>-58:20:33.4</t>
+  </si>
+  <si>
+    <t>-55:59:03.92</t>
+  </si>
+  <si>
+    <t>-64:07:53.91</t>
+  </si>
+  <si>
+    <t>-64:08:43</t>
+  </si>
+  <si>
     <t>-64:23:23.85</t>
   </si>
   <si>
+    <t>-58:20:40.89</t>
+  </si>
+  <si>
+    <t>-66:17:21.8</t>
+  </si>
+  <si>
+    <t>-35:12:26.0</t>
+  </si>
+  <si>
     <t>-58:59:29.1</t>
   </si>
   <si>
+    <t>-64:08:43.8</t>
+  </si>
+  <si>
     <t>-67:00:49.2</t>
   </si>
   <si>
     <t>-62:22:44.6</t>
   </si>
   <si>
+    <t>-63:01:15.39</t>
+  </si>
+  <si>
+    <t>-43:57:44.12</t>
+  </si>
+  <si>
+    <t>-62:04:18.7</t>
+  </si>
+  <si>
     <t>-62:28</t>
   </si>
   <si>
     <t>-60:38:08.0</t>
   </si>
   <si>
+    <t>-63:57:45.54</t>
+  </si>
+  <si>
+    <t>-74:04:53.32</t>
+  </si>
+  <si>
+    <t>-55:30:50.2</t>
+  </si>
+  <si>
     <t>-66:23:05.04</t>
   </si>
   <si>
+    <t>-60:36:31.35</t>
+  </si>
+  <si>
     <t>-64:13:15.59</t>
   </si>
   <si>
     <t>-68:43:39.25</t>
   </si>
   <si>
+    <t>-57:59:59.8</t>
+  </si>
+  <si>
+    <t>-58:29:02.7</t>
+  </si>
+  <si>
+    <t>-53:34:19.3</t>
+  </si>
+  <si>
+    <t>-56:26:25.4</t>
+  </si>
+  <si>
+    <t>-53:08:46.5</t>
+  </si>
+  <si>
+    <t>-42:58:12.66</t>
+  </si>
+  <si>
     <t>-44:38:45.901778</t>
   </si>
   <si>
     <t>-50:44:20.96</t>
   </si>
   <si>
+    <t>-51:00:06.1</t>
+  </si>
+  <si>
+    <t>-49:09:58.34</t>
+  </si>
+  <si>
     <t>-52:57:34.5</t>
   </si>
   <si>
+    <t>-52:09:23.6</t>
+  </si>
+  <si>
+    <t>-50:48:03.5</t>
+  </si>
+  <si>
+    <t>-47:33:05.0</t>
+  </si>
+  <si>
+    <t>-44:53:07.8</t>
+  </si>
+  <si>
+    <t>-50:15:08.1</t>
+  </si>
+  <si>
+    <t>-12:24:58.6831</t>
+  </si>
+  <si>
     <t>-45:59:09.5</t>
   </si>
   <si>
+    <t>-68:31:51</t>
+  </si>
+  <si>
     <t>-42:46:11</t>
   </si>
   <si>
+    <t>-52:22:58.2</t>
+  </si>
+  <si>
+    <t>-52:55:48</t>
+  </si>
+  <si>
+    <t>-38:38:20.8</t>
+  </si>
+  <si>
+    <t>-37:26:25</t>
+  </si>
+  <si>
+    <t>-32:41:48.0373</t>
+  </si>
+  <si>
+    <t>-48:51:55.8</t>
+  </si>
+  <si>
+    <t>-34:23:45.17</t>
+  </si>
+  <si>
     <t>-40:53:56.1</t>
   </si>
   <si>
+    <t>-47:29:34.5</t>
+  </si>
+  <si>
     <t>-16:40:57.73</t>
   </si>
   <si>
     <t>-44:29:08.24</t>
   </si>
   <si>
+    <t>-34:24:59.5684</t>
+  </si>
+  <si>
     <t>-35:32:49.6144</t>
   </si>
   <si>
+    <t>-32:07:45.3326</t>
+  </si>
+  <si>
+    <t>-37:12:03.7</t>
+  </si>
+  <si>
+    <t>-33:50:39.4333</t>
+  </si>
+  <si>
     <t>-47:44:34.56</t>
   </si>
   <si>
+    <t>-37:16:55.23</t>
+  </si>
+  <si>
+    <t>-32:11:53.6471</t>
+  </si>
+  <si>
+    <t>-29:03:03.4825</t>
+  </si>
+  <si>
+    <t>-31:31:15.3012</t>
+  </si>
+  <si>
+    <t>-30:15:43.5</t>
+  </si>
+  <si>
+    <t>-39:27:38.0</t>
+  </si>
+  <si>
     <t>-11:34:54.68126</t>
   </si>
   <si>
     <t>-30:40:23.19</t>
   </si>
   <si>
+    <t>-31:57:44.1409</t>
+  </si>
+  <si>
+    <t>-33:23:39.6</t>
+  </si>
+  <si>
+    <t>-46:57:24.8</t>
+  </si>
+  <si>
     <t>-28:06:37.3</t>
   </si>
   <si>
+    <t>-24:22:07.4457</t>
+  </si>
+  <si>
+    <t>-21:37:07.351</t>
+  </si>
+  <si>
+    <t>-36:18:04.0</t>
+  </si>
+  <si>
+    <t>-38:37:59.7</t>
+  </si>
+  <si>
+    <t>-14:22:36.71</t>
+  </si>
+  <si>
+    <t>-22:56:30.6089</t>
+  </si>
+  <si>
+    <t>-31:06:49.7498</t>
+  </si>
+  <si>
+    <t>-19:45:51.7164</t>
+  </si>
+  <si>
+    <t>-13:34:46.8</t>
+  </si>
+  <si>
     <t>-17:51:03.8981</t>
   </si>
   <si>
+    <t>-10:59:27.926</t>
+  </si>
+  <si>
+    <t>-10:08:08.3481</t>
+  </si>
+  <si>
     <t>-26:00:43.8</t>
   </si>
   <si>
+    <t>-26:02:05.75</t>
+  </si>
+  <si>
     <t>-16:16:44.55350</t>
+  </si>
+  <si>
+    <t>-72:00:42.2</t>
+  </si>
+  <si>
+    <t>-52:36:36.2260</t>
+  </si>
+  <si>
+    <t>-20:05:29.63</t>
   </si>
 </sst>
 </file>
@@ -678,7 +1533,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -689,22 +1544,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>264</v>
       </c>
       <c r="D1">
-        <v>0.005757451936712637</v>
+        <v>0.1369616105136507</v>
       </c>
       <c r="E1">
-        <v>0.141</v>
+        <v>1.9</v>
       </c>
       <c r="F1">
-        <v>160</v>
+        <v>3.9</v>
       </c>
       <c r="G1">
-        <v>2.64476</v>
+        <v>21.806</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -712,22 +1567,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>265</v>
       </c>
       <c r="D2">
-        <v>0.5489392232937018</v>
+        <v>0.447708444058</v>
       </c>
       <c r="E2">
-        <v>26.8</v>
+        <v>7.5</v>
       </c>
       <c r="F2">
-        <v>16.8</v>
+        <v>5</v>
       </c>
       <c r="G2">
-        <v>39.903</v>
+        <v>15.9</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -735,22 +1590,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>266</v>
       </c>
       <c r="D3">
-        <v>1.244418596151246</v>
+        <v>0.5452527423520001</v>
       </c>
       <c r="E3">
-        <v>63.3</v>
+        <v>20.3</v>
       </c>
       <c r="F3">
-        <v>31.9</v>
+        <v>3.8</v>
       </c>
       <c r="G3">
-        <v>34.425</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -758,22 +1613,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>135</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>267</v>
       </c>
       <c r="D4">
-        <v>0.374919985032</v>
+        <v>0.005757451936712637</v>
       </c>
       <c r="E4">
-        <v>22.7</v>
+        <v>0.141</v>
       </c>
       <c r="F4">
-        <v>99.7</v>
+        <v>160</v>
       </c>
       <c r="G4">
-        <v>160.896</v>
+        <v>2.64476</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -781,22 +1636,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>268</v>
       </c>
       <c r="D5">
-        <v>0.1667622915721636</v>
+        <v>0.5489392232937018</v>
       </c>
       <c r="E5">
-        <v>4.2</v>
+        <v>26.8</v>
       </c>
       <c r="F5">
-        <v>26</v>
+        <v>16.8</v>
       </c>
       <c r="G5">
-        <v>73.72799999999999</v>
+        <v>39.903</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -804,22 +1659,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>79</v>
+        <v>269</v>
       </c>
       <c r="D6">
-        <v>0.08932838502359318</v>
+        <v>1.24585559629</v>
       </c>
       <c r="E6">
-        <v>1.4</v>
+        <v>57.1</v>
       </c>
       <c r="F6">
-        <v>1050</v>
+        <v>8.4</v>
       </c>
       <c r="G6">
-        <v>67.97</v>
+        <v>18.58</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -827,22 +1682,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>270</v>
       </c>
       <c r="D7">
-        <v>0.7516236176460001</v>
+        <v>1.244418596151246</v>
       </c>
       <c r="E7">
-        <v>4.4</v>
+        <v>63.3</v>
       </c>
       <c r="F7">
-        <v>35</v>
+        <v>31.9</v>
       </c>
       <c r="G7">
-        <v>147.29</v>
+        <v>34.425</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -850,22 +1705,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>139</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>271</v>
       </c>
       <c r="D8">
-        <v>0.253556015011</v>
+        <v>1.22475441462</v>
       </c>
       <c r="E8">
-        <v>12.1</v>
+        <v>13.3</v>
       </c>
       <c r="F8">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="G8">
-        <v>103.72</v>
+        <v>32.39</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -873,22 +1728,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>272</v>
       </c>
       <c r="D9">
-        <v>0.1067545925</v>
+        <v>0.5101603448262563</v>
       </c>
       <c r="E9">
-        <v>0.9</v>
+        <v>5.5</v>
       </c>
       <c r="F9">
-        <v>20</v>
+        <v>1.9</v>
       </c>
       <c r="G9">
-        <v>180.37</v>
+        <v>61.293</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -896,22 +1751,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>141</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>273</v>
       </c>
       <c r="D10">
-        <v>0.66436748807</v>
+        <v>0.374919985032</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>22.7</v>
       </c>
       <c r="F10">
-        <v>11</v>
+        <v>99.7</v>
       </c>
       <c r="G10">
-        <v>180.2</v>
+        <v>160.896</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -919,22 +1774,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>274</v>
       </c>
       <c r="D11">
-        <v>0.422447188684</v>
+        <v>0.1667622915721636</v>
       </c>
       <c r="E11">
-        <v>17.4</v>
+        <v>4.2</v>
       </c>
       <c r="F11">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G11">
-        <v>320.3</v>
+        <v>73.72799999999999</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -942,22 +1797,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>85</v>
+        <v>275</v>
       </c>
       <c r="D12">
-        <v>0.40052204834</v>
+        <v>0.2148363514</v>
       </c>
       <c r="E12">
-        <v>11.3</v>
+        <v>10.7</v>
       </c>
       <c r="F12">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G12">
-        <v>325.2</v>
+        <v>121.38</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -965,22 +1820,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>144</v>
       </c>
       <c r="C13" t="s">
-        <v>86</v>
+        <v>276</v>
       </c>
       <c r="D13">
-        <v>0.388480921041</v>
+        <v>0.6822651758059591</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="F13">
-        <v>34.2</v>
+        <v>2.6</v>
       </c>
       <c r="G13">
-        <v>297.25</v>
+        <v>63.327</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -988,22 +1843,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>277</v>
       </c>
       <c r="D14">
-        <v>0.47799086689</v>
+        <v>0.547199235502</v>
       </c>
       <c r="E14">
-        <v>5.6</v>
+        <v>8.1</v>
       </c>
       <c r="F14">
-        <v>18</v>
+        <v>2.6</v>
       </c>
       <c r="G14">
-        <v>287.3</v>
+        <v>228.3</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1011,22 +1866,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>278</v>
       </c>
       <c r="D15">
-        <v>0.5430085792</v>
+        <v>1.238129543868176</v>
       </c>
       <c r="E15">
-        <v>41.9</v>
+        <v>21.7</v>
       </c>
       <c r="F15">
-        <v>13.6</v>
+        <v>6</v>
       </c>
       <c r="G15">
-        <v>209.6</v>
+        <v>40.938</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1034,22 +1889,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>147</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>279</v>
       </c>
       <c r="D16">
-        <v>0.5299131921</v>
+        <v>0.08932838502359318</v>
       </c>
       <c r="E16">
-        <v>8.800000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="F16">
-        <v>21</v>
+        <v>1050</v>
       </c>
       <c r="G16">
-        <v>318.8</v>
+        <v>67.97</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1057,22 +1912,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>148</v>
       </c>
       <c r="C17" t="s">
-        <v>90</v>
+        <v>280</v>
       </c>
       <c r="D17">
-        <v>0.455761</v>
+        <v>0.7516236176460001</v>
       </c>
       <c r="E17">
-        <v>18.2</v>
+        <v>4.4</v>
       </c>
       <c r="F17">
-        <v>13.2</v>
+        <v>35</v>
       </c>
       <c r="G17">
-        <v>416.8</v>
+        <v>147.29</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1080,22 +1935,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>149</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>281</v>
       </c>
       <c r="D18">
-        <v>0.12750077685</v>
+        <v>1.116097163401556</v>
       </c>
       <c r="E18">
-        <v>2.5</v>
+        <v>18.6</v>
       </c>
       <c r="F18">
-        <v>12.5</v>
+        <v>5</v>
       </c>
       <c r="G18">
-        <v>293.736</v>
+        <v>94.16</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1103,22 +1958,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>282</v>
       </c>
       <c r="D19">
-        <v>0.785440757324</v>
+        <v>0.9625085573</v>
       </c>
       <c r="E19">
-        <v>3.9</v>
+        <v>16.8</v>
       </c>
       <c r="F19">
-        <v>16.3</v>
+        <v>3.3</v>
       </c>
       <c r="G19">
-        <v>65.3</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1126,22 +1981,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="C20" t="s">
-        <v>93</v>
+        <v>283</v>
       </c>
       <c r="D20">
-        <v>0.1794847539641</v>
+        <v>0.253556015011</v>
       </c>
       <c r="E20">
-        <v>3.1</v>
+        <v>12.1</v>
       </c>
       <c r="F20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G20">
-        <v>71.248</v>
+        <v>103.72</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1149,22 +2004,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>152</v>
       </c>
       <c r="C21" t="s">
-        <v>94</v>
+        <v>284</v>
       </c>
       <c r="D21">
-        <v>0.2633768148933</v>
+        <v>0.4016256234421612</v>
       </c>
       <c r="E21">
-        <v>12.4</v>
+        <v>8.6</v>
       </c>
       <c r="F21">
-        <v>64.2</v>
+        <v>4</v>
       </c>
       <c r="G21">
-        <v>8.638999999999999</v>
+        <v>15.879</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1172,22 +2027,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>153</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>285</v>
       </c>
       <c r="D22">
-        <v>0.2570560976508</v>
+        <v>0.1067545925</v>
       </c>
       <c r="E22">
-        <v>6.5</v>
+        <v>0.9</v>
       </c>
       <c r="F22">
-        <v>37.1</v>
+        <v>20</v>
       </c>
       <c r="G22">
-        <v>56.1</v>
+        <v>180.37</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1195,22 +2050,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>154</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>286</v>
       </c>
       <c r="D23">
-        <v>0.1926012327811</v>
+        <v>1.3628899542</v>
       </c>
       <c r="E23">
-        <v>4.3</v>
+        <v>13.3</v>
       </c>
       <c r="F23">
-        <v>21</v>
+        <v>1.9</v>
       </c>
       <c r="G23">
-        <v>262.791</v>
+        <v>54.3</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1218,22 +2073,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>155</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>287</v>
       </c>
       <c r="D24">
-        <v>0.6580131007</v>
+        <v>0.73950132654</v>
       </c>
       <c r="E24">
-        <v>59.8</v>
+        <v>40.5</v>
       </c>
       <c r="F24">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="G24">
-        <v>35.1</v>
+        <v>57.4</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1241,22 +2096,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>61</v>
+        <v>156</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>288</v>
       </c>
       <c r="D25">
-        <v>0.455059775403</v>
+        <v>1.44477320982</v>
       </c>
       <c r="E25">
-        <v>8</v>
+        <v>22.5</v>
       </c>
       <c r="F25">
-        <v>300</v>
+        <v>3.2</v>
       </c>
       <c r="G25">
-        <v>478.8</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1264,22 +2119,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>289</v>
       </c>
       <c r="D26">
-        <v>0.84408066596</v>
+        <v>0.66436748807</v>
       </c>
       <c r="E26">
-        <v>102.2</v>
+        <v>9</v>
       </c>
       <c r="F26">
-        <v>21.4</v>
+        <v>11</v>
       </c>
       <c r="G26">
-        <v>482</v>
+        <v>180.2</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1287,22 +2142,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>158</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>290</v>
       </c>
       <c r="D27">
-        <v>0.58101670786</v>
+        <v>1.3738151214</v>
       </c>
       <c r="E27">
-        <v>30.7</v>
+        <v>33.6</v>
       </c>
       <c r="F27">
-        <v>10.2</v>
+        <v>4</v>
       </c>
       <c r="G27">
-        <v>360</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1310,22 +2165,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
+        <v>291</v>
       </c>
       <c r="D28">
-        <v>0.6530539712555028</v>
+        <v>1.4365826292</v>
       </c>
       <c r="E28">
-        <v>7.6</v>
+        <v>7.2</v>
       </c>
       <c r="F28">
-        <v>14.5</v>
+        <v>10</v>
       </c>
       <c r="G28">
-        <v>24.891</v>
+        <v>130.32</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1333,22 +2188,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>160</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>292</v>
       </c>
       <c r="D29">
-        <v>0.102459245929448</v>
+        <v>0.8199114962</v>
       </c>
       <c r="E29">
-        <v>5.7</v>
+        <v>7.3</v>
       </c>
       <c r="F29">
-        <v>12.1</v>
+        <v>1.8</v>
       </c>
       <c r="G29">
-        <v>75.68000000000001</v>
+        <v>383.9</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1356,22 +2211,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>293</v>
       </c>
       <c r="D30">
-        <v>0.2804238585494842</v>
+        <v>0.442900630729</v>
       </c>
       <c r="E30">
-        <v>29.8</v>
+        <v>4.3</v>
       </c>
       <c r="F30">
-        <v>16.8</v>
+        <v>2.6</v>
       </c>
       <c r="G30">
-        <v>496</v>
+        <v>379.78</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1379,22 +2234,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>294</v>
       </c>
       <c r="D31">
-        <v>0.8298287852354905</v>
+        <v>0.50345881546</v>
       </c>
       <c r="E31">
-        <v>17.1</v>
+        <v>2.9</v>
       </c>
       <c r="F31">
-        <v>27</v>
+        <v>1.8</v>
       </c>
       <c r="G31">
-        <v>123.056</v>
+        <v>438.7</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1402,22 +2257,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>163</v>
       </c>
       <c r="C32" t="s">
-        <v>105</v>
+        <v>295</v>
       </c>
       <c r="D32">
-        <v>0.00407454594143919</v>
+        <v>0.1984514505627</v>
       </c>
       <c r="E32">
-        <v>0.137</v>
+        <v>2.2</v>
       </c>
       <c r="F32">
-        <v>13</v>
+        <v>3.1</v>
       </c>
       <c r="G32">
-        <v>3.13695</v>
+        <v>116.156</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1425,22 +2280,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>69</v>
+        <v>164</v>
       </c>
       <c r="C33" t="s">
-        <v>106</v>
+        <v>296</v>
       </c>
       <c r="D33">
-        <v>0.3674324514817157</v>
+        <v>0.1236706578868608</v>
       </c>
       <c r="E33">
-        <v>6.1</v>
+        <v>4.8</v>
       </c>
       <c r="F33">
-        <v>21</v>
+        <v>9.1</v>
       </c>
       <c r="G33">
-        <v>88.373</v>
+        <v>128.679</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1448,22 +2303,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>165</v>
       </c>
       <c r="C34" t="s">
-        <v>107</v>
+        <v>297</v>
       </c>
       <c r="D34">
-        <v>0.5625576355342506</v>
+        <v>0.422447188684</v>
       </c>
       <c r="E34">
-        <v>6.1</v>
+        <v>17.4</v>
       </c>
       <c r="F34">
-        <v>47.8</v>
+        <v>34</v>
       </c>
       <c r="G34">
-        <v>50.372</v>
+        <v>320.3</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1471,22 +2326,22 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>166</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>298</v>
       </c>
       <c r="D35">
-        <v>0.3071329758225554</v>
+        <v>0.558252726401</v>
       </c>
       <c r="E35">
-        <v>13.5</v>
+        <v>20.2</v>
       </c>
       <c r="F35">
-        <v>11</v>
+        <v>3.3</v>
       </c>
       <c r="G35">
-        <v>217.108</v>
+        <v>262.56</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1494,22 +2349,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>167</v>
       </c>
       <c r="C36" t="s">
-        <v>109</v>
+        <v>299</v>
       </c>
       <c r="D36">
-        <v>0.6122092044382964</v>
+        <v>0.88081962549</v>
       </c>
       <c r="E36">
-        <v>52</v>
+        <v>27.4</v>
       </c>
       <c r="F36">
-        <v>15</v>
+        <v>4.7</v>
       </c>
       <c r="G36">
-        <v>37.994</v>
+        <v>677</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1517,22 +2372,2207 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>168</v>
+      </c>
+      <c r="C37" t="s">
+        <v>300</v>
+      </c>
+      <c r="D37">
+        <v>0.943157882843</v>
+      </c>
+      <c r="E37">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="F37">
+        <v>6</v>
+      </c>
+      <c r="G37">
+        <v>40.53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" t="s">
+        <v>301</v>
+      </c>
+      <c r="D38">
+        <v>0.50509714918</v>
+      </c>
+      <c r="E38">
+        <v>3.9</v>
+      </c>
+      <c r="F38">
+        <v>1.6</v>
+      </c>
+      <c r="G38">
+        <v>493.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>170</v>
+      </c>
+      <c r="C39" t="s">
+        <v>302</v>
+      </c>
+      <c r="D39">
+        <v>0.36470557624</v>
+      </c>
+      <c r="E39">
+        <v>13.6</v>
+      </c>
+      <c r="F39">
+        <v>6</v>
+      </c>
+      <c r="G39">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>171</v>
+      </c>
+      <c r="C40" t="s">
+        <v>303</v>
+      </c>
+      <c r="D40">
+        <v>0.3938988148377834</v>
+      </c>
+      <c r="E40">
+        <v>4.4</v>
+      </c>
+      <c r="F40">
+        <v>2.4</v>
+      </c>
+      <c r="G40">
+        <v>116.08</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>172</v>
+      </c>
+      <c r="C41" t="s">
+        <v>304</v>
+      </c>
+      <c r="D41">
+        <v>0.40052204834</v>
+      </c>
+      <c r="E41">
+        <v>11.3</v>
+      </c>
+      <c r="F41">
+        <v>14</v>
+      </c>
+      <c r="G41">
+        <v>325.2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>173</v>
+      </c>
+      <c r="C42" t="s">
+        <v>305</v>
+      </c>
+      <c r="D42">
+        <v>0.452800508195</v>
+      </c>
+      <c r="E42">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="F42">
+        <v>3</v>
+      </c>
+      <c r="G42">
+        <v>145.41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>174</v>
+      </c>
+      <c r="C43" t="s">
+        <v>306</v>
+      </c>
+      <c r="D43">
+        <v>0.2797673308446</v>
+      </c>
+      <c r="E43">
+        <v>4.7</v>
+      </c>
+      <c r="F43">
+        <v>2.3</v>
+      </c>
+      <c r="G43">
+        <v>174.347</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>175</v>
+      </c>
+      <c r="C44" t="s">
+        <v>307</v>
+      </c>
+      <c r="D44">
+        <v>0.2164762031209</v>
+      </c>
+      <c r="E44">
+        <v>5.5</v>
+      </c>
+      <c r="F44">
+        <v>8.9</v>
+      </c>
+      <c r="G44">
+        <v>97.68600000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>176</v>
+      </c>
+      <c r="C45" t="s">
+        <v>308</v>
+      </c>
+      <c r="D45">
+        <v>0.4196177915</v>
+      </c>
+      <c r="E45">
+        <v>4.5</v>
+      </c>
+      <c r="F45">
+        <v>1.8</v>
+      </c>
+      <c r="G45">
+        <v>415.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>177</v>
+      </c>
+      <c r="C46" t="s">
+        <v>309</v>
+      </c>
+      <c r="D46">
+        <v>0.388480921041</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46">
+        <v>34.2</v>
+      </c>
+      <c r="G46">
+        <v>297.25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>178</v>
+      </c>
+      <c r="C47" t="s">
+        <v>310</v>
+      </c>
+      <c r="D47">
+        <v>0.2554963274098</v>
+      </c>
+      <c r="E47">
+        <v>3.5</v>
+      </c>
+      <c r="F47">
+        <v>4.1</v>
+      </c>
+      <c r="G47">
+        <v>100.584</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>179</v>
+      </c>
+      <c r="C48" t="s">
+        <v>311</v>
+      </c>
+      <c r="D48">
+        <v>0.473026470689</v>
+      </c>
+      <c r="E48">
+        <v>20.4</v>
+      </c>
+      <c r="F48">
+        <v>5</v>
+      </c>
+      <c r="G48">
+        <v>436.9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>180</v>
+      </c>
+      <c r="C49" t="s">
+        <v>312</v>
+      </c>
+      <c r="D49">
+        <v>0.45848840672</v>
+      </c>
+      <c r="E49">
+        <v>9.800000000000001</v>
+      </c>
+      <c r="F49">
+        <v>4.7</v>
+      </c>
+      <c r="G49">
+        <v>16.42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>181</v>
+      </c>
+      <c r="C50" t="s">
+        <v>313</v>
+      </c>
+      <c r="D50">
+        <v>0.47799086689</v>
+      </c>
+      <c r="E50">
+        <v>5.6</v>
+      </c>
+      <c r="F50">
+        <v>18</v>
+      </c>
+      <c r="G50">
+        <v>287.3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>182</v>
+      </c>
+      <c r="C51" t="s">
+        <v>314</v>
+      </c>
+      <c r="D51">
+        <v>0.7926701073</v>
+      </c>
+      <c r="E51">
+        <v>7.7</v>
+      </c>
+      <c r="F51">
+        <v>1.9</v>
+      </c>
+      <c r="G51">
+        <v>502.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>183</v>
+      </c>
+      <c r="C52" t="s">
+        <v>315</v>
+      </c>
+      <c r="D52">
+        <v>0.5430085792</v>
+      </c>
+      <c r="E52">
+        <v>41.9</v>
+      </c>
+      <c r="F52">
+        <v>13.6</v>
+      </c>
+      <c r="G52">
+        <v>209.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>184</v>
+      </c>
+      <c r="C53" t="s">
+        <v>316</v>
+      </c>
+      <c r="D53">
+        <v>0.5299131921</v>
+      </c>
+      <c r="E53">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="F53">
+        <v>21</v>
+      </c>
+      <c r="G53">
+        <v>318.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" t="s">
+        <v>317</v>
+      </c>
+      <c r="D54">
+        <v>0.196478664183</v>
+      </c>
+      <c r="E54">
+        <v>4.8</v>
+      </c>
+      <c r="F54">
+        <v>4.2</v>
+      </c>
+      <c r="G54">
+        <v>294.91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>186</v>
+      </c>
+      <c r="C55" t="s">
+        <v>318</v>
+      </c>
+      <c r="D55">
+        <v>0.53269880337</v>
+      </c>
+      <c r="E55">
+        <v>10.4</v>
+      </c>
+      <c r="F55">
+        <v>4.4</v>
+      </c>
+      <c r="G55">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>187</v>
+      </c>
+      <c r="C56" t="s">
+        <v>319</v>
+      </c>
+      <c r="D56">
+        <v>1.2389895765</v>
+      </c>
+      <c r="E56">
+        <v>89.5</v>
+      </c>
+      <c r="F56">
+        <v>5.9</v>
+      </c>
+      <c r="G56">
+        <v>640.3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>188</v>
+      </c>
+      <c r="C57" t="s">
+        <v>320</v>
+      </c>
+      <c r="D57">
+        <v>0.455761</v>
+      </c>
+      <c r="E57">
+        <v>18.2</v>
+      </c>
+      <c r="F57">
+        <v>13.2</v>
+      </c>
+      <c r="G57">
+        <v>416.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>189</v>
+      </c>
+      <c r="C58" t="s">
+        <v>321</v>
+      </c>
+      <c r="D58">
+        <v>0.12750077685</v>
+      </c>
+      <c r="E58">
+        <v>2.5</v>
+      </c>
+      <c r="F58">
+        <v>12.5</v>
+      </c>
+      <c r="G58">
+        <v>293.736</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>190</v>
+      </c>
+      <c r="C59" t="s">
+        <v>322</v>
+      </c>
+      <c r="D59">
+        <v>0.84278963237</v>
+      </c>
+      <c r="E59">
+        <v>9.1</v>
+      </c>
+      <c r="F59">
+        <v>7.1</v>
+      </c>
+      <c r="G59">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>191</v>
+      </c>
+      <c r="C60" t="s">
+        <v>323</v>
+      </c>
+      <c r="D60">
+        <v>0.2787294436271</v>
+      </c>
+      <c r="E60">
+        <v>1.1</v>
+      </c>
+      <c r="F60">
+        <v>1.2</v>
+      </c>
+      <c r="G60">
+        <v>54.24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>192</v>
+      </c>
+      <c r="C61" t="s">
+        <v>324</v>
+      </c>
+      <c r="D61">
+        <v>0.570290462862</v>
+      </c>
+      <c r="E61">
+        <v>12.2</v>
+      </c>
+      <c r="F61">
+        <v>6.5</v>
+      </c>
+      <c r="G61">
+        <v>82.40000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>193</v>
+      </c>
+      <c r="C62" t="s">
+        <v>325</v>
+      </c>
+      <c r="D62">
+        <v>0.785440757324</v>
+      </c>
+      <c r="E62">
+        <v>3.9</v>
+      </c>
+      <c r="F62">
+        <v>16.3</v>
+      </c>
+      <c r="G62">
+        <v>65.3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>194</v>
+      </c>
+      <c r="C63" t="s">
+        <v>326</v>
+      </c>
+      <c r="D63">
+        <v>0.1549913579183</v>
+      </c>
+      <c r="E63">
+        <v>1.5</v>
+      </c>
+      <c r="F63">
+        <v>1.9</v>
+      </c>
+      <c r="G63">
+        <v>349.54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>195</v>
+      </c>
+      <c r="C64" t="s">
+        <v>327</v>
+      </c>
+      <c r="D64">
+        <v>0.1794847539641</v>
+      </c>
+      <c r="E64">
+        <v>3.1</v>
+      </c>
+      <c r="F64">
+        <v>18</v>
+      </c>
+      <c r="G64">
+        <v>71.248</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>196</v>
+      </c>
+      <c r="C65" t="s">
+        <v>328</v>
+      </c>
+      <c r="D65">
+        <v>0.2633768148933</v>
+      </c>
+      <c r="E65">
+        <v>12.4</v>
+      </c>
+      <c r="F65">
+        <v>64.2</v>
+      </c>
+      <c r="G65">
+        <v>8.638999999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>197</v>
+      </c>
+      <c r="C66" t="s">
+        <v>329</v>
+      </c>
+      <c r="D66">
+        <v>0.128694148448</v>
+      </c>
+      <c r="E66">
+        <v>4.9</v>
+      </c>
+      <c r="F66">
+        <v>7.8</v>
+      </c>
+      <c r="G66">
+        <v>627.47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>198</v>
+      </c>
+      <c r="C67" t="s">
+        <v>330</v>
+      </c>
+      <c r="D67">
+        <v>0.395352859901</v>
+      </c>
+      <c r="E67">
+        <v>13.2</v>
+      </c>
+      <c r="F67">
+        <v>6</v>
+      </c>
+      <c r="G67">
+        <v>199.9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>199</v>
+      </c>
+      <c r="C68" t="s">
+        <v>331</v>
+      </c>
+      <c r="D68">
+        <v>1.36888090921</v>
+      </c>
+      <c r="E68">
+        <v>12.2</v>
+      </c>
+      <c r="F68">
+        <v>6.8</v>
+      </c>
+      <c r="G68">
+        <v>24.82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>200</v>
+      </c>
+      <c r="C69" t="s">
+        <v>332</v>
+      </c>
+      <c r="D69">
+        <v>0.2433922004</v>
+      </c>
+      <c r="E69">
+        <v>7.6</v>
+      </c>
+      <c r="F69">
+        <v>5</v>
+      </c>
+      <c r="G69">
+        <v>175.85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>201</v>
+      </c>
+      <c r="C70" t="s">
+        <v>333</v>
+      </c>
+      <c r="D70">
+        <v>0.178553799688</v>
+      </c>
+      <c r="E70">
+        <v>4</v>
+      </c>
+      <c r="F70">
+        <v>5</v>
+      </c>
+      <c r="G70">
+        <v>35.16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>202</v>
+      </c>
+      <c r="C71" t="s">
+        <v>334</v>
+      </c>
+      <c r="D71">
+        <v>0.329186857758</v>
+      </c>
+      <c r="E71">
+        <v>3.8</v>
+      </c>
+      <c r="F71">
+        <v>2.7</v>
+      </c>
+      <c r="G71">
+        <v>144.497</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>203</v>
+      </c>
+      <c r="C72" t="s">
+        <v>335</v>
+      </c>
+      <c r="D72">
+        <v>0.2570560976508</v>
+      </c>
+      <c r="E72">
+        <v>6.5</v>
+      </c>
+      <c r="F72">
+        <v>37.1</v>
+      </c>
+      <c r="G72">
+        <v>56.1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>204</v>
+      </c>
+      <c r="C73" t="s">
+        <v>336</v>
+      </c>
+      <c r="D73">
+        <v>0.1926012327811</v>
+      </c>
+      <c r="E73">
+        <v>4.3</v>
+      </c>
+      <c r="F73">
+        <v>21</v>
+      </c>
+      <c r="G73">
+        <v>262.791</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
         <v>73</v>
       </c>
-      <c r="C37" t="s">
+      <c r="B74" t="s">
+        <v>205</v>
+      </c>
+      <c r="C74" t="s">
+        <v>337</v>
+      </c>
+      <c r="D74">
+        <v>0.86422735995</v>
+      </c>
+      <c r="E74">
+        <v>4.3</v>
+      </c>
+      <c r="F74">
+        <v>7</v>
+      </c>
+      <c r="G74">
+        <v>170.79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>206</v>
+      </c>
+      <c r="C75" t="s">
+        <v>338</v>
+      </c>
+      <c r="D75">
+        <v>0.327417572788</v>
+      </c>
+      <c r="E75">
+        <v>3.8</v>
+      </c>
+      <c r="F75">
+        <v>6.1</v>
+      </c>
+      <c r="G75">
+        <v>140.8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>207</v>
+      </c>
+      <c r="C76" t="s">
+        <v>339</v>
+      </c>
+      <c r="D76">
+        <v>0.6580131007</v>
+      </c>
+      <c r="E76">
+        <v>59.8</v>
+      </c>
+      <c r="F76">
+        <v>21</v>
+      </c>
+      <c r="G76">
+        <v>35.1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>208</v>
+      </c>
+      <c r="C77" t="s">
+        <v>340</v>
+      </c>
+      <c r="D77">
+        <v>0.182491659288</v>
+      </c>
+      <c r="E77">
+        <v>1.1</v>
+      </c>
+      <c r="F77">
+        <v>1.45</v>
+      </c>
+      <c r="G77">
+        <v>127.345</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>209</v>
+      </c>
+      <c r="C78" t="s">
+        <v>341</v>
+      </c>
+      <c r="D78">
+        <v>0.2316938362300844</v>
+      </c>
+      <c r="E78">
+        <v>8.4</v>
+      </c>
+      <c r="F78">
+        <v>4.1</v>
+      </c>
+      <c r="G78">
+        <v>582.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>210</v>
+      </c>
+      <c r="C79" t="s">
+        <v>342</v>
+      </c>
+      <c r="D79">
+        <v>0.57597141155</v>
+      </c>
+      <c r="E79">
+        <v>82.7</v>
+      </c>
+      <c r="F79">
+        <v>9.9</v>
+      </c>
+      <c r="G79">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>211</v>
+      </c>
+      <c r="C80" t="s">
+        <v>343</v>
+      </c>
+      <c r="D80">
+        <v>0.436506697158</v>
+      </c>
+      <c r="E80">
+        <v>7.6</v>
+      </c>
+      <c r="F80">
+        <v>2.6</v>
+      </c>
+      <c r="G80">
+        <v>474.1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>212</v>
+      </c>
+      <c r="C81" t="s">
+        <v>344</v>
+      </c>
+      <c r="D81">
+        <v>0.352142380018</v>
+      </c>
+      <c r="E81">
+        <v>6.2</v>
+      </c>
+      <c r="F81">
+        <v>7.6</v>
+      </c>
+      <c r="G81">
+        <v>398.41</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>213</v>
+      </c>
+      <c r="C82" t="s">
+        <v>345</v>
+      </c>
+      <c r="D82">
+        <v>0.00462164152493627</v>
+      </c>
+      <c r="E82">
+        <v>0.314</v>
+      </c>
+      <c r="F82">
+        <v>4.8</v>
+      </c>
+      <c r="G82">
+        <v>62.4143</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>214</v>
+      </c>
+      <c r="C83" t="s">
+        <v>346</v>
+      </c>
+      <c r="D83">
+        <v>0.455059775403</v>
+      </c>
+      <c r="E83">
+        <v>8</v>
+      </c>
+      <c r="F83">
+        <v>300</v>
+      </c>
+      <c r="G83">
+        <v>478.8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>215</v>
+      </c>
+      <c r="C84" t="s">
+        <v>347</v>
+      </c>
+      <c r="D84">
+        <v>1.7856112396</v>
+      </c>
+      <c r="E84">
+        <v>74.90000000000001</v>
+      </c>
+      <c r="F84">
+        <v>4.9</v>
+      </c>
+      <c r="G84">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>216</v>
+      </c>
+      <c r="C85" t="s">
+        <v>348</v>
+      </c>
+      <c r="D85">
+        <v>0.84408066596</v>
+      </c>
+      <c r="E85">
+        <v>102.2</v>
+      </c>
+      <c r="F85">
+        <v>21.4</v>
+      </c>
+      <c r="G85">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>217</v>
+      </c>
+      <c r="C86" t="s">
+        <v>349</v>
+      </c>
+      <c r="D86">
+        <v>0.63505597647</v>
+      </c>
+      <c r="E86">
+        <v>16.1</v>
+      </c>
+      <c r="F86">
+        <v>4.1</v>
+      </c>
+      <c r="G86">
+        <v>179.1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>218</v>
+      </c>
+      <c r="C87" t="s">
+        <v>350</v>
+      </c>
+      <c r="D87">
+        <v>0.8905339578</v>
+      </c>
+      <c r="E87">
+        <v>20.8</v>
+      </c>
+      <c r="F87">
+        <v>3.3</v>
+      </c>
+      <c r="G87">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>219</v>
+      </c>
+      <c r="C88" t="s">
+        <v>351</v>
+      </c>
+      <c r="D88">
+        <v>0.305037318882</v>
+      </c>
+      <c r="E88">
+        <v>2.4</v>
+      </c>
+      <c r="F88">
+        <v>2</v>
+      </c>
+      <c r="G88">
+        <v>207.2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>220</v>
+      </c>
+      <c r="C89" t="s">
+        <v>352</v>
+      </c>
+      <c r="D89">
+        <v>2.4546091591</v>
+      </c>
+      <c r="E89">
+        <v>40.9</v>
+      </c>
+      <c r="F89">
+        <v>4.1</v>
+      </c>
+      <c r="G89">
+        <v>303.4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>221</v>
+      </c>
+      <c r="C90" t="s">
+        <v>353</v>
+      </c>
+      <c r="D90">
+        <v>1.211785094646978</v>
+      </c>
+      <c r="E90">
+        <v>37.7</v>
+      </c>
+      <c r="F90">
+        <v>8.699999999999999</v>
+      </c>
+      <c r="G90">
+        <v>110.306</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>222</v>
+      </c>
+      <c r="C91" t="s">
+        <v>354</v>
+      </c>
+      <c r="D91">
+        <v>1.39640107763</v>
+      </c>
+      <c r="E91">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="F91">
+        <v>1.4</v>
+      </c>
+      <c r="G91">
+        <v>150.29</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>223</v>
+      </c>
+      <c r="C92" t="s">
+        <v>355</v>
+      </c>
+      <c r="D92">
+        <v>0.2554264836009563</v>
+      </c>
+      <c r="E92">
+        <v>11.7</v>
+      </c>
+      <c r="F92">
+        <v>5.3</v>
+      </c>
+      <c r="G92">
+        <v>146.36</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>224</v>
+      </c>
+      <c r="C93" t="s">
+        <v>356</v>
+      </c>
+      <c r="D93">
+        <v>0.58101670786</v>
+      </c>
+      <c r="E93">
+        <v>30.7</v>
+      </c>
+      <c r="F93">
+        <v>10.2</v>
+      </c>
+      <c r="G93">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>225</v>
+      </c>
+      <c r="C94" t="s">
+        <v>357</v>
+      </c>
+      <c r="D94">
+        <v>0.26647363743</v>
+      </c>
+      <c r="E94">
+        <v>4.7</v>
+      </c>
+      <c r="F94">
+        <v>2.4</v>
+      </c>
+      <c r="G94">
+        <v>268.3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>226</v>
+      </c>
+      <c r="C95" t="s">
+        <v>358</v>
+      </c>
+      <c r="D95">
+        <v>0.6530539712555028</v>
+      </c>
+      <c r="E95">
+        <v>7.6</v>
+      </c>
+      <c r="F95">
+        <v>14.5</v>
+      </c>
+      <c r="G95">
+        <v>24.891</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>227</v>
+      </c>
+      <c r="C96" t="s">
+        <v>359</v>
+      </c>
+      <c r="D96">
+        <v>0.102459245929448</v>
+      </c>
+      <c r="E96">
+        <v>5.7</v>
+      </c>
+      <c r="F96">
+        <v>12.1</v>
+      </c>
+      <c r="G96">
+        <v>75.68000000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>228</v>
+      </c>
+      <c r="C97" t="s">
+        <v>360</v>
+      </c>
+      <c r="D97">
+        <v>0.6562992314590905</v>
+      </c>
+      <c r="E97">
+        <v>11.5</v>
+      </c>
+      <c r="F97">
+        <v>3.9</v>
+      </c>
+      <c r="G97">
+        <v>587.7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>229</v>
+      </c>
+      <c r="C98" t="s">
+        <v>361</v>
+      </c>
+      <c r="D98">
+        <v>0.2804238585494842</v>
+      </c>
+      <c r="E98">
+        <v>29.8</v>
+      </c>
+      <c r="F98">
+        <v>16.8</v>
+      </c>
+      <c r="G98">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>230</v>
+      </c>
+      <c r="C99" t="s">
+        <v>362</v>
+      </c>
+      <c r="D99">
+        <v>0.477157518355834</v>
+      </c>
+      <c r="E99">
+        <v>5.2</v>
+      </c>
+      <c r="F99">
+        <v>5.4</v>
+      </c>
+      <c r="G99">
+        <v>126.064</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>231</v>
+      </c>
+      <c r="C100" t="s">
+        <v>363</v>
+      </c>
+      <c r="D100">
+        <v>0.236173191636</v>
+      </c>
+      <c r="E100">
+        <v>3.7</v>
+      </c>
+      <c r="F100">
+        <v>3.8</v>
+      </c>
+      <c r="G100">
+        <v>99.48999999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>232</v>
+      </c>
+      <c r="C101" t="s">
+        <v>364</v>
+      </c>
+      <c r="D101">
+        <v>0.1394602112498516</v>
+      </c>
+      <c r="E101">
+        <v>7.1</v>
+      </c>
+      <c r="F101">
+        <v>4.3</v>
+      </c>
+      <c r="G101">
+        <v>261.29</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+      <c r="B102" t="s">
+        <v>233</v>
+      </c>
+      <c r="C102" t="s">
+        <v>365</v>
+      </c>
+      <c r="D102">
+        <v>0.8298287852354905</v>
+      </c>
+      <c r="E102">
+        <v>17.1</v>
+      </c>
+      <c r="F102">
+        <v>27</v>
+      </c>
+      <c r="G102">
+        <v>123.056</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103" t="s">
+        <v>234</v>
+      </c>
+      <c r="C103" t="s">
+        <v>366</v>
+      </c>
+      <c r="D103">
+        <v>0.3375936984807235</v>
+      </c>
+      <c r="E103">
+        <v>3.9</v>
+      </c>
+      <c r="F103">
+        <v>3.6</v>
+      </c>
+      <c r="G103">
+        <v>153.18</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" t="s">
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>235</v>
+      </c>
+      <c r="C104" t="s">
+        <v>367</v>
+      </c>
+      <c r="D104">
+        <v>0.7684989454804679</v>
+      </c>
+      <c r="E104">
+        <v>11.3</v>
+      </c>
+      <c r="F104">
+        <v>2.4</v>
+      </c>
+      <c r="G104">
+        <v>49.59</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+      <c r="B105" t="s">
+        <v>236</v>
+      </c>
+      <c r="C105" t="s">
+        <v>368</v>
+      </c>
+      <c r="D105">
+        <v>0.322882431773582</v>
+      </c>
+      <c r="E105">
+        <v>6</v>
+      </c>
+      <c r="F105">
+        <v>4.5</v>
+      </c>
+      <c r="G105">
+        <v>138.55</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" t="s">
+        <v>105</v>
+      </c>
+      <c r="B106" t="s">
+        <v>237</v>
+      </c>
+      <c r="C106" t="s">
+        <v>369</v>
+      </c>
+      <c r="D106">
+        <v>0.5294409884251815</v>
+      </c>
+      <c r="E106">
+        <v>20.7</v>
+      </c>
+      <c r="F106">
+        <v>6.2</v>
+      </c>
+      <c r="G106">
+        <v>600.1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" t="s">
+        <v>106</v>
+      </c>
+      <c r="B107" t="s">
+        <v>238</v>
+      </c>
+      <c r="C107" t="s">
+        <v>370</v>
+      </c>
+      <c r="D107">
+        <v>0.6068866242543225</v>
+      </c>
+      <c r="E107">
+        <v>2.4</v>
+      </c>
+      <c r="F107">
+        <v>8.9</v>
+      </c>
+      <c r="G107">
+        <v>151.96</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" t="s">
+        <v>107</v>
+      </c>
+      <c r="B108" t="s">
+        <v>239</v>
+      </c>
+      <c r="C108" t="s">
+        <v>371</v>
+      </c>
+      <c r="D108">
+        <v>0.512211401067</v>
+      </c>
+      <c r="E108">
+        <v>10.5</v>
+      </c>
+      <c r="F108">
+        <v>5.5</v>
+      </c>
+      <c r="G108">
+        <v>158.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" t="s">
+        <v>108</v>
+      </c>
+      <c r="B109" t="s">
+        <v>240</v>
+      </c>
+      <c r="C109" t="s">
+        <v>372</v>
+      </c>
+      <c r="D109">
+        <v>0.00407454594143919</v>
+      </c>
+      <c r="E109">
+        <v>0.137</v>
+      </c>
+      <c r="F109">
+        <v>13</v>
+      </c>
+      <c r="G109">
+        <v>3.13695</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110" t="s">
+        <v>241</v>
+      </c>
+      <c r="C110" t="s">
+        <v>373</v>
+      </c>
+      <c r="D110">
+        <v>0.3674324514817157</v>
+      </c>
+      <c r="E110">
+        <v>6.1</v>
+      </c>
+      <c r="F110">
+        <v>21</v>
+      </c>
+      <c r="G110">
+        <v>88.373</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
         <v>110</v>
       </c>
-      <c r="D37">
+      <c r="B111" t="s">
+        <v>242</v>
+      </c>
+      <c r="C111" t="s">
+        <v>374</v>
+      </c>
+      <c r="D111">
+        <v>0.9103629841498471</v>
+      </c>
+      <c r="E111">
+        <v>7.1</v>
+      </c>
+      <c r="F111">
+        <v>1.7</v>
+      </c>
+      <c r="G111">
+        <v>206.34</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" t="s">
+        <v>111</v>
+      </c>
+      <c r="B112" t="s">
+        <v>243</v>
+      </c>
+      <c r="C112" t="s">
+        <v>375</v>
+      </c>
+      <c r="D112">
+        <v>0.5482271037961444</v>
+      </c>
+      <c r="E112">
+        <v>5.9</v>
+      </c>
+      <c r="F112">
+        <v>1.9</v>
+      </c>
+      <c r="G112">
+        <v>296.7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+      <c r="B113" t="s">
+        <v>244</v>
+      </c>
+      <c r="C113" t="s">
+        <v>376</v>
+      </c>
+      <c r="D113">
+        <v>0.74235239547</v>
+      </c>
+      <c r="E113">
+        <v>11.5</v>
+      </c>
+      <c r="F113">
+        <v>6.6</v>
+      </c>
+      <c r="G113">
+        <v>20.4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" t="s">
+        <v>113</v>
+      </c>
+      <c r="B114" t="s">
+        <v>245</v>
+      </c>
+      <c r="C114" t="s">
+        <v>377</v>
+      </c>
+      <c r="D114">
+        <v>0.5625576355342506</v>
+      </c>
+      <c r="E114">
+        <v>6.1</v>
+      </c>
+      <c r="F114">
+        <v>47.8</v>
+      </c>
+      <c r="G114">
+        <v>50.372</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>246</v>
+      </c>
+      <c r="C115" t="s">
+        <v>378</v>
+      </c>
+      <c r="D115">
+        <v>0.2341057912524572</v>
+      </c>
+      <c r="E115">
+        <v>9.6</v>
+      </c>
+      <c r="F115">
+        <v>7.2</v>
+      </c>
+      <c r="G115">
+        <v>179.454</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" t="s">
+        <v>115</v>
+      </c>
+      <c r="B116" t="s">
+        <v>247</v>
+      </c>
+      <c r="C116" t="s">
+        <v>379</v>
+      </c>
+      <c r="D116">
+        <v>0.1336669202502843</v>
+      </c>
+      <c r="E116">
+        <v>13.1</v>
+      </c>
+      <c r="F116">
+        <v>9.6</v>
+      </c>
+      <c r="G116">
+        <v>233.99</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+      <c r="B117" t="s">
+        <v>248</v>
+      </c>
+      <c r="C117" t="s">
+        <v>380</v>
+      </c>
+      <c r="D117">
+        <v>0.38701692095</v>
+      </c>
+      <c r="E117">
+        <v>9</v>
+      </c>
+      <c r="F117">
+        <v>3.2</v>
+      </c>
+      <c r="G117">
+        <v>94.3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" t="s">
+        <v>117</v>
+      </c>
+      <c r="B118" t="s">
+        <v>249</v>
+      </c>
+      <c r="C118" t="s">
+        <v>381</v>
+      </c>
+      <c r="D118">
+        <v>0.38448678392</v>
+      </c>
+      <c r="E118">
+        <v>4.5</v>
+      </c>
+      <c r="F118">
+        <v>3.1</v>
+      </c>
+      <c r="G118">
+        <v>102.847</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" t="s">
+        <v>118</v>
+      </c>
+      <c r="B119" t="s">
+        <v>250</v>
+      </c>
+      <c r="C119" t="s">
+        <v>382</v>
+      </c>
+      <c r="D119">
+        <v>0.2914894606391399</v>
+      </c>
+      <c r="E119">
+        <v>17.1</v>
+      </c>
+      <c r="F119">
+        <v>9.6</v>
+      </c>
+      <c r="G119">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" t="s">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>251</v>
+      </c>
+      <c r="C120" t="s">
+        <v>383</v>
+      </c>
+      <c r="D120">
+        <v>1.874268518251891</v>
+      </c>
+      <c r="E120">
+        <v>43.7</v>
+      </c>
+      <c r="F120">
+        <v>3.8</v>
+      </c>
+      <c r="G120">
+        <v>121.2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" t="s">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>252</v>
+      </c>
+      <c r="C121" t="s">
+        <v>384</v>
+      </c>
+      <c r="D121">
+        <v>0.284054344966819</v>
+      </c>
+      <c r="E121">
+        <v>3.6</v>
+      </c>
+      <c r="F121">
+        <v>5.6</v>
+      </c>
+      <c r="G121">
+        <v>50.245</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" t="s">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>253</v>
+      </c>
+      <c r="C122" t="s">
+        <v>385</v>
+      </c>
+      <c r="D122">
+        <v>0.1893349899448201</v>
+      </c>
+      <c r="E122">
+        <v>1.3</v>
+      </c>
+      <c r="F122">
+        <v>7.8</v>
+      </c>
+      <c r="G122">
+        <v>224.38</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
+      <c r="A123" t="s">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>254</v>
+      </c>
+      <c r="C123" t="s">
+        <v>386</v>
+      </c>
+      <c r="D123">
+        <v>0.1014867942075943</v>
+      </c>
+      <c r="E123">
+        <v>5.9</v>
+      </c>
+      <c r="F123">
+        <v>4.7</v>
+      </c>
+      <c r="G123">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
+      <c r="A124" t="s">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>255</v>
+      </c>
+      <c r="C124" t="s">
+        <v>387</v>
+      </c>
+      <c r="D124">
+        <v>0.3071329758225554</v>
+      </c>
+      <c r="E124">
+        <v>13.5</v>
+      </c>
+      <c r="F124">
+        <v>11</v>
+      </c>
+      <c r="G124">
+        <v>217.108</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
+      <c r="A125" t="s">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>256</v>
+      </c>
+      <c r="C125" t="s">
+        <v>388</v>
+      </c>
+      <c r="D125">
+        <v>0.4050433216298211</v>
+      </c>
+      <c r="E125">
+        <v>2</v>
+      </c>
+      <c r="F125">
+        <v>1.5</v>
+      </c>
+      <c r="G125">
+        <v>159.7</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
+      <c r="A126" t="s">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>257</v>
+      </c>
+      <c r="C126" t="s">
+        <v>389</v>
+      </c>
+      <c r="D126">
+        <v>0.5627107361360836</v>
+      </c>
+      <c r="E126">
+        <v>6.1</v>
+      </c>
+      <c r="F126">
+        <v>4.8</v>
+      </c>
+      <c r="G126">
+        <v>316.98</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
+      <c r="A127" t="s">
+        <v>126</v>
+      </c>
+      <c r="B127" t="s">
+        <v>258</v>
+      </c>
+      <c r="C127" t="s">
+        <v>390</v>
+      </c>
+      <c r="D127">
+        <v>0.6122092044382964</v>
+      </c>
+      <c r="E127">
+        <v>52</v>
+      </c>
+      <c r="F127">
+        <v>15</v>
+      </c>
+      <c r="G127">
+        <v>37.994</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" t="s">
+        <v>127</v>
+      </c>
+      <c r="B128" t="s">
+        <v>259</v>
+      </c>
+      <c r="C128" t="s">
+        <v>391</v>
+      </c>
+      <c r="D128">
+        <v>0.4028579088754282</v>
+      </c>
+      <c r="E128">
+        <v>3.1</v>
+      </c>
+      <c r="F128">
+        <v>1.9</v>
+      </c>
+      <c r="G128">
+        <v>50.036</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" t="s">
+        <v>128</v>
+      </c>
+      <c r="B129" t="s">
+        <v>260</v>
+      </c>
+      <c r="C129" t="s">
+        <v>392</v>
+      </c>
+      <c r="D129">
         <v>1.961572303612613</v>
       </c>
-      <c r="E37">
+      <c r="E129">
         <v>9.800000000000001</v>
       </c>
-      <c r="F37">
+      <c r="F129">
         <v>22</v>
       </c>
-      <c r="G37">
+      <c r="G129">
         <v>11.456</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" t="s">
+        <v>129</v>
+      </c>
+      <c r="B130" t="s">
+        <v>261</v>
+      </c>
+      <c r="C130" t="s">
+        <v>393</v>
+      </c>
+      <c r="D130">
+        <v>0.341336231373</v>
+      </c>
+      <c r="E130">
+        <v>24.4</v>
+      </c>
+      <c r="F130">
+        <v>6</v>
+      </c>
+      <c r="G130">
+        <v>17.3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" t="s">
+        <v>130</v>
+      </c>
+      <c r="B131" t="s">
+        <v>262</v>
+      </c>
+      <c r="C131" t="s">
+        <v>394</v>
+      </c>
+      <c r="D131">
+        <v>0.002186699771552793</v>
+      </c>
+      <c r="E131">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F131">
+        <v>4.1</v>
+      </c>
+      <c r="G131">
+        <v>11.41085</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
+      <c r="A132" t="s">
+        <v>131</v>
+      </c>
+      <c r="B132" t="s">
+        <v>263</v>
+      </c>
+      <c r="C132" t="s">
+        <v>395</v>
+      </c>
+      <c r="D132">
+        <v>1.643622185326949</v>
+      </c>
+      <c r="E132">
+        <v>6.4</v>
+      </c>
+      <c r="F132">
+        <v>2.9</v>
+      </c>
+      <c r="G132">
+        <v>8.456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>